<commit_message>
Change the key to robert.
</commit_message>
<xml_diff>
--- a/athena-doc/Restful服务框架(Athena) - 开发计划.xlsx
+++ b/athena-doc/Restful服务框架(Athena) - 开发计划.xlsx
@@ -116,10 +116,6 @@
     <t>Q2</t>
   </si>
   <si>
-    <t>李艳鹏</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Sprint Q2.R2
 2015/4/10-2015/4/23</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -180,39 +176,6 @@
   </si>
   <si>
     <t>环境属性管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>与</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>DCMD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>模板集成</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -289,10 +252,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>考虑类似Tair和注册中心的版本控制原理，实现服务注册和客户端负载均衡，与王鹏谈论中</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>改造框架项目中的athena-rest-comm项目使用apache io或者nio2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -331,6 +290,37 @@
   </si>
   <si>
     <t>Q3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>罗伯特</t>
+  </si>
+  <si>
+    <t>考虑类似Tair和注册中心的版本控制原理，实现服务注册和客户端负载均衡，与爱丽丝谈论中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>与上线流程</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>集成</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -534,7 +524,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -585,9 +575,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -612,24 +621,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -970,58 +963,58 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="27">
       <c r="A4" s="4" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1110,7 +1103,7 @@
     </row>
     <row r="1048576" spans="3:4">
       <c r="C1048576" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1048576" s="4" t="s">
         <v>22</v>
@@ -1163,43 +1156,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="23" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="21" t="s">
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="28" t="s">
         <v>6</v>
       </c>
       <c r="L1" s="5"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="22"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="21"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="28"/>
       <c r="H2" s="7" t="s">
         <v>2</v>
       </c>
@@ -1209,24 +1202,24 @@
       <c r="J2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="22"/>
+      <c r="K2" s="29"/>
       <c r="L2" s="5"/>
     </row>
     <row r="3" spans="1:12" ht="40.5">
       <c r="A3" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="4">
         <v>3</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>10</v>
@@ -1235,13 +1228,13 @@
         <v>11</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>7</v>
@@ -1252,18 +1245,18 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="27">
-      <c r="A4" s="20"/>
-      <c r="B4" s="30" t="s">
-        <v>34</v>
+      <c r="A4" s="26"/>
+      <c r="B4" s="22" t="s">
+        <v>33</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" s="4">
         <v>3</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>9</v>
@@ -1272,13 +1265,13 @@
         <v>11</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>7</v>
@@ -1289,16 +1282,16 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="20"/>
-      <c r="B5" s="32"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="4">
         <v>2</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>10</v>
@@ -1307,13 +1300,13 @@
         <v>11</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>7</v>
@@ -1324,31 +1317,31 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="20"/>
-      <c r="B6" s="31"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="4">
         <v>2</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>7</v>
@@ -1376,19 +1369,19 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>36</v>
+        <v>25</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>35</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="4">
         <v>2</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>10</v>
@@ -1397,13 +1390,13 @@
         <v>11</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>7</v>
@@ -1412,30 +1405,30 @@
     </row>
     <row r="9" spans="1:12" ht="13.5" customHeight="1">
       <c r="A9" s="18"/>
-      <c r="B9" s="31"/>
+      <c r="B9" s="24"/>
       <c r="C9" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="4">
         <v>2</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>7</v>
@@ -1444,17 +1437,17 @@
     </row>
     <row r="10" spans="1:12" ht="13.5" customHeight="1">
       <c r="A10" s="18"/>
-      <c r="B10" s="30" t="s">
-        <v>42</v>
+      <c r="B10" s="22" t="s">
+        <v>40</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="4">
         <v>2</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>10</v>
@@ -1463,13 +1456,13 @@
         <v>11</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>7</v>
@@ -1478,15 +1471,15 @@
     </row>
     <row r="11" spans="1:12" ht="13.5" customHeight="1">
       <c r="A11" s="18"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="4" t="s">
-        <v>40</v>
+      <c r="B11" s="23"/>
+      <c r="C11" s="36" t="s">
+        <v>63</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>10</v>
@@ -1495,13 +1488,13 @@
         <v>11</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>7</v>
@@ -1510,15 +1503,15 @@
     </row>
     <row r="12" spans="1:12" ht="13.5" customHeight="1">
       <c r="A12" s="18"/>
-      <c r="B12" s="31"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D12" s="4">
         <v>3</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>9</v>
@@ -1527,13 +1520,13 @@
         <v>11</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>7</v>
@@ -1561,19 +1554,19 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="30" t="s">
-        <v>61</v>
+        <v>26</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>58</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" s="4">
         <v>5</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>10</v>
@@ -1582,13 +1575,13 @@
         <v>11</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>7</v>
@@ -1597,15 +1590,15 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="18"/>
-      <c r="B15" s="29"/>
+      <c r="B15" s="25"/>
       <c r="C15" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="9">
         <v>5</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>9</v>
@@ -1614,13 +1607,13 @@
         <v>11</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>7</v>
@@ -1650,31 +1643,31 @@
         <v>19</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>7</v>
@@ -1683,17 +1676,17 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="18"/>
-      <c r="B18" s="34" t="s">
-        <v>36</v>
+      <c r="B18" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D18" s="4">
         <v>5</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>9</v>
@@ -1702,13 +1695,13 @@
         <v>11</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>7</v>
@@ -1717,15 +1710,15 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="18"/>
-      <c r="B19" s="35"/>
+      <c r="B19" s="21"/>
       <c r="C19" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D19" s="4">
         <v>4</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>9</v>
@@ -1734,13 +1727,13 @@
         <v>11</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>7</v>
@@ -1767,17 +1760,17 @@
       <c r="A21" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="34" t="s">
-        <v>56</v>
+      <c r="B21" s="20" t="s">
+        <v>53</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D21" s="4">
         <v>5</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>9</v>
@@ -1786,13 +1779,13 @@
         <v>11</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>7</v>
@@ -1801,15 +1794,15 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="18"/>
-      <c r="B22" s="35"/>
+      <c r="B22" s="21"/>
       <c r="C22" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D22" s="4">
         <v>5</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>10</v>
@@ -1818,13 +1811,13 @@
         <v>11</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K22" s="4" t="s">
         <v>7</v>
@@ -1852,34 +1845,34 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="30" t="s">
-        <v>57</v>
+        <v>59</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>54</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D24" s="4">
         <v>4</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K24" s="4" t="s">
         <v>7</v>
@@ -1887,31 +1880,31 @@
       <c r="L24" s="16"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="20"/>
-      <c r="B25" s="32"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D25" s="4">
         <v>5</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K25" s="4" t="s">
         <v>7</v>
@@ -1919,31 +1912,31 @@
       <c r="L25" s="16"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="20"/>
-      <c r="B26" s="31"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="24"/>
       <c r="C26" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D26" s="4">
         <v>1</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>7</v>
@@ -1951,7 +1944,7 @@
       <c r="L26" s="16"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="33"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="5"/>
       <c r="C27" s="11" t="s">
         <v>21</v>
@@ -2087,14 +2080,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A24:A27"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="K1:K2"/>
@@ -2108,6 +2093,14 @@
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A24:A27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">

</xml_diff>